<commit_message>
Changes on the auto evaluation files.
</commit_message>
<xml_diff>
--- a/docs/SprintC/Grelha Auto Avaliação - Sprint C.xlsx
+++ b/docs/SprintC/Grelha Auto Avaliação - Sprint C.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myisepipp-my.sharepoint.com/personal/1211076_isep_ipp_pt/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guga\OneDrive\Documentos\lei-22-s2-1da-g02\docs\SprintC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="84" documentId="13_ncr:1_{6967B764-8B0A-48B6-ADA7-0FB940204365}" xr6:coauthVersionLast="48" xr6:coauthVersionMax="48" xr10:uidLastSave="{2B7CDEC8-FA90-4703-8364-CF58FF45B4A6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E18E6565-72C1-4DAA-8737-A5F0FEA2876C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="48" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="1" xr2:uid="{5633927D-80FC-C741-B738-D107B2C827F5}"/>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="1" xr2:uid="{CBF4613B-34B8-DA4D-9F7C-C401008AD6A5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{5633927D-80FC-C741-B738-D107B2C827F5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{CBF4613B-34B8-DA4D-9F7C-C401008AD6A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Group and Self Assessment" sheetId="17" r:id="rId1"/>
@@ -250,7 +250,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -303,6 +303,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -723,7 +731,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -884,6 +892,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1104,7 +1113,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1405,7 +1414,7 @@
     <sheetView workbookViewId="0"/>
     <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="5.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
@@ -1413,25 +1422,25 @@
     <col min="20" max="20" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="21">
+    <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
         <v>2</v>
       </c>
@@ -1440,13 +1449,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="16.5" thickBot="1"/>
-    <row r="8" spans="1:20" ht="15.95" customHeight="1" thickBot="1">
+    <row r="7" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:20" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
       <c r="E8" s="53" t="s">
@@ -1468,7 +1477,7 @@
       <c r="S8" s="54"/>
       <c r="T8" s="55"/>
     </row>
-    <row r="9" spans="1:20" ht="105.95" customHeight="1" thickBot="1">
+    <row r="9" spans="1:20" ht="105.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
       <c r="D9" s="24" t="str">
@@ -1535,7 +1544,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="16.5" thickBot="1">
+    <row r="10" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="56" t="s">
         <v>7</v>
       </c>
@@ -1562,7 +1571,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="16.5" thickBot="1">
+    <row r="11" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="57"/>
       <c r="C11" s="41" t="s">
         <v>9</v>
@@ -1587,7 +1596,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="16.5" thickBot="1">
+    <row r="12" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="57"/>
       <c r="C12" s="41" t="s">
         <v>10</v>
@@ -1612,7 +1621,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="16.5" thickBot="1">
+    <row r="13" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="57"/>
       <c r="C13" s="41" t="s">
         <v>11</v>
@@ -1637,7 +1646,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="16.5" thickBot="1">
+    <row r="14" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="57"/>
       <c r="C14" s="41" t="s">
         <v>12</v>
@@ -1662,7 +1671,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="16.5" thickBot="1">
+    <row r="15" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="57"/>
       <c r="C15" s="41" t="s">
         <v>13</v>
@@ -1687,7 +1696,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="16.5" thickBot="1">
+    <row r="16" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="57"/>
       <c r="C16" s="41" t="s">
         <v>14</v>
@@ -1712,7 +1721,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="16.5" thickBot="1">
+    <row r="17" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="57"/>
       <c r="C17" s="41" t="s">
         <v>15</v>
@@ -1737,7 +1746,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="16.5" thickBot="1">
+    <row r="18" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="57"/>
       <c r="C18" s="41" t="s">
         <v>16</v>
@@ -1762,7 +1771,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="16.5" thickBot="1">
+    <row r="19" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="57"/>
       <c r="C19" s="41" t="s">
         <v>17</v>
@@ -1787,7 +1796,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="16.5" thickBot="1">
+    <row r="20" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="57"/>
       <c r="C20" s="41" t="s">
         <v>18</v>
@@ -1812,7 +1821,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="16.5" thickBot="1">
+    <row r="21" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="57"/>
       <c r="C21" s="41" t="s">
         <v>19</v>
@@ -1837,7 +1846,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="16.5" thickBot="1">
+    <row r="22" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="57"/>
       <c r="C22" s="41" t="s">
         <v>20</v>
@@ -1862,7 +1871,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="16.5" thickBot="1">
+    <row r="23" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="57"/>
       <c r="C23" s="41" t="s">
         <v>21</v>
@@ -1887,7 +1896,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="16.5" thickBot="1">
+    <row r="24" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="58"/>
       <c r="C24" s="46" t="s">
         <v>22</v>
@@ -1912,7 +1921,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="16.5" thickBot="1">
+    <row r="25" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="22"/>
       <c r="C25" s="30" t="s">
         <v>6</v>
@@ -1979,27 +1988,27 @@
       </c>
       <c r="S25" s="33"/>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:19">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:19">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="34" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:19">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:19">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>0</v>
       </c>
@@ -2007,7 +2016,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:19">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
@@ -2015,7 +2024,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2</v>
       </c>
@@ -2023,7 +2032,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>3</v>
       </c>
@@ -2031,7 +2040,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>4</v>
       </c>
@@ -2039,7 +2048,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>5</v>
       </c>
@@ -2067,17 +2076,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F15ACC4-0801-A246-B800-FA1501AC2D32}">
   <dimension ref="A1:Y123"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="X3" sqref="X3:Y8"/>
+      <selection pane="bottomLeft" activeCell="X3" sqref="X3:Y8"/>
       <selection pane="bottomRight" activeCell="A3" sqref="A3:A8"/>
-      <selection pane="bottomLeft" activeCell="X3" sqref="X3:Y8"/>
-      <selection pane="topRight" activeCell="X3" sqref="X3:Y8"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="1">
-      <selection activeCell="S14" sqref="S14"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="1">
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" style="2"/>
     <col min="2" max="2" width="11" style="2" customWidth="1"/>
@@ -2094,7 +2103,7 @@
     <col min="25" max="25" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" ht="409.5">
+    <row r="1" spans="1:25" s="1" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>33</v>
       </c>
@@ -2161,7 +2170,7 @@
       </c>
       <c r="Y1" s="3"/>
     </row>
-    <row r="2" spans="1:25" s="1" customFormat="1">
+    <row r="2" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>52</v>
       </c>
@@ -2239,7 +2248,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="62" t="s">
         <v>60</v>
       </c>
@@ -2313,7 +2322,7 @@
       </c>
       <c r="Y3" s="49"/>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="62"/>
       <c r="B4" s="51">
         <v>1211061</v>
@@ -2385,7 +2394,7 @@
       </c>
       <c r="Y4" s="49"/>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="62"/>
       <c r="B5" s="51">
         <v>1211073</v>
@@ -2457,7 +2466,7 @@
       </c>
       <c r="Y5" s="49"/>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="62"/>
       <c r="B6" s="51">
         <v>1211063</v>
@@ -2502,13 +2511,13 @@
         <v>4.5</v>
       </c>
       <c r="P6" s="49">
+        <v>3.75</v>
+      </c>
+      <c r="Q6" s="49">
+        <v>4</v>
+      </c>
+      <c r="R6" s="49">
         <v>4.5</v>
-      </c>
-      <c r="Q6" s="49">
-        <v>3.5</v>
-      </c>
-      <c r="R6" s="49">
-        <v>4</v>
       </c>
       <c r="S6" s="49">
         <v>4</v>
@@ -2518,18 +2527,18 @@
       </c>
       <c r="V6" s="6">
         <f t="shared" si="0"/>
-        <v>82</v>
+        <v>82.625</v>
       </c>
       <c r="W6" s="7">
         <f t="shared" si="1"/>
-        <v>16.399999999999999</v>
+        <v>16.53</v>
       </c>
       <c r="X6" s="49">
         <v>16</v>
       </c>
       <c r="Y6" s="49"/>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="62"/>
       <c r="B7" s="51">
         <v>1211076</v>
@@ -2582,7 +2591,7 @@
       <c r="R7" s="49">
         <v>4</v>
       </c>
-      <c r="S7" s="49">
+      <c r="S7" s="64">
         <v>4</v>
       </c>
       <c r="T7" s="49">
@@ -2601,7 +2610,7 @@
       </c>
       <c r="Y7" s="49"/>
     </row>
-    <row r="8" spans="1:25" ht="16.5" thickBot="1">
+    <row r="8" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="63"/>
       <c r="B8" s="52"/>
       <c r="C8" s="16" t="str">
@@ -2640,7 +2649,7 @@
       <c r="X8" s="50"/>
       <c r="Y8" s="50"/>
     </row>
-    <row r="9" spans="1:25" ht="16.5" thickTop="1">
+    <row r="9" spans="1:25" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="59"/>
       <c r="C9" s="5" t="str">
         <f>IFERROR(VLOOKUP(B9,#REF!,2,FALSE),"")</f>
@@ -2659,7 +2668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="60"/>
       <c r="C10" s="5" t="str">
         <f>IFERROR(VLOOKUP(B10,#REF!,2,FALSE),"")</f>
@@ -2678,7 +2687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="60"/>
       <c r="C11" s="5" t="str">
         <f>IFERROR(VLOOKUP(B11,#REF!,2,FALSE),"")</f>
@@ -2697,7 +2706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="60"/>
       <c r="C12" s="5" t="str">
         <f>IFERROR(VLOOKUP(B12,#REF!,2,FALSE),"")</f>
@@ -2716,7 +2725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="60"/>
       <c r="C13" s="5" t="str">
         <f>IFERROR(VLOOKUP(B13,#REF!,2,FALSE),"")</f>
@@ -2735,7 +2744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="16.5" thickBot="1">
+    <row r="14" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="61"/>
       <c r="B14" s="15"/>
       <c r="C14" s="16" t="str">
@@ -2774,7 +2783,7 @@
       <c r="X14" s="14"/>
       <c r="Y14" s="14"/>
     </row>
-    <row r="15" spans="1:25" ht="16.5" thickTop="1">
+    <row r="15" spans="1:25" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A15" s="59"/>
       <c r="C15" s="5" t="str">
         <f>IFERROR(VLOOKUP(B15,#REF!,2,FALSE),"")</f>
@@ -2793,7 +2802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="60"/>
       <c r="C16" s="5" t="str">
         <f>IFERROR(VLOOKUP(B16,#REF!,2,FALSE),"")</f>
@@ -2812,7 +2821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="60"/>
       <c r="C17" s="5" t="str">
         <f>IFERROR(VLOOKUP(B17,#REF!,2,FALSE),"")</f>
@@ -2831,7 +2840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="60"/>
       <c r="C18" s="5" t="str">
         <f>IFERROR(VLOOKUP(B18,#REF!,2,FALSE),"")</f>
@@ -2850,7 +2859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="60"/>
       <c r="C19" s="5" t="str">
         <f>IFERROR(VLOOKUP(B19,#REF!,2,FALSE),"")</f>
@@ -2869,7 +2878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="16.5" thickBot="1">
+    <row r="20" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="61"/>
       <c r="B20" s="15"/>
       <c r="C20" s="16" t="str">
@@ -2908,7 +2917,7 @@
       <c r="X20" s="14"/>
       <c r="Y20" s="14"/>
     </row>
-    <row r="21" spans="1:25" ht="16.5" thickTop="1">
+    <row r="21" spans="1:25" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A21" s="59"/>
       <c r="C21" s="5" t="str">
         <f>IFERROR(VLOOKUP(B21,#REF!,2,FALSE),"")</f>
@@ -2927,7 +2936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="60"/>
       <c r="C22" s="5" t="str">
         <f>IFERROR(VLOOKUP(B22,#REF!,2,FALSE),"")</f>
@@ -2946,7 +2955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="60"/>
       <c r="C23" s="5" t="str">
         <f>IFERROR(VLOOKUP(B23,#REF!,2,FALSE),"")</f>
@@ -2965,7 +2974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="60"/>
       <c r="C24" s="5" t="str">
         <f>IFERROR(VLOOKUP(B24,#REF!,2,FALSE),"")</f>
@@ -2984,7 +2993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="60"/>
       <c r="C25" s="5" t="str">
         <f>IFERROR(VLOOKUP(B25,#REF!,2,FALSE),"")</f>
@@ -3003,7 +3012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:25" ht="16.5" thickBot="1">
+    <row r="26" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="61"/>
       <c r="B26" s="15"/>
       <c r="C26" s="16" t="str">
@@ -3042,7 +3051,7 @@
       <c r="X26" s="14"/>
       <c r="Y26" s="14"/>
     </row>
-    <row r="27" spans="1:25" ht="16.5" thickTop="1">
+    <row r="27" spans="1:25" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A27" s="59"/>
       <c r="C27" s="5" t="str">
         <f>IFERROR(VLOOKUP(B27,#REF!,2,FALSE),"")</f>
@@ -3061,7 +3070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" s="60"/>
       <c r="C28" s="5" t="str">
         <f>IFERROR(VLOOKUP(B28,#REF!,2,FALSE),"")</f>
@@ -3080,7 +3089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" s="60"/>
       <c r="C29" s="5" t="str">
         <f>IFERROR(VLOOKUP(B29,#REF!,2,FALSE),"")</f>
@@ -3099,7 +3108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" s="60"/>
       <c r="C30" s="5" t="str">
         <f>IFERROR(VLOOKUP(B30,#REF!,2,FALSE),"")</f>
@@ -3118,7 +3127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" s="60"/>
       <c r="C31" s="5" t="str">
         <f>IFERROR(VLOOKUP(B31,#REF!,2,FALSE),"")</f>
@@ -3137,7 +3146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:25" ht="16.5" thickBot="1">
+    <row r="32" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="61"/>
       <c r="B32" s="15"/>
       <c r="C32" s="16" t="str">
@@ -3176,7 +3185,7 @@
       <c r="X32" s="14"/>
       <c r="Y32" s="14"/>
     </row>
-    <row r="33" spans="1:25" ht="16.5" thickTop="1">
+    <row r="33" spans="1:25" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A33" s="59"/>
       <c r="C33" s="5" t="str">
         <f>IFERROR(VLOOKUP(B33,#REF!,2,FALSE),"")</f>
@@ -3195,7 +3204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" s="60"/>
       <c r="C34" s="5" t="str">
         <f>IFERROR(VLOOKUP(B34,#REF!,2,FALSE),"")</f>
@@ -3214,7 +3223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" s="60"/>
       <c r="C35" s="5" t="str">
         <f>IFERROR(VLOOKUP(B35,#REF!,2,FALSE),"")</f>
@@ -3233,7 +3242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" s="60"/>
       <c r="C36" s="5" t="str">
         <f>IFERROR(VLOOKUP(B36,#REF!,2,FALSE),"")</f>
@@ -3252,7 +3261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" s="60"/>
       <c r="C37" s="5" t="str">
         <f>IFERROR(VLOOKUP(B37,#REF!,2,FALSE),"")</f>
@@ -3271,7 +3280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:25" ht="16.5" thickBot="1">
+    <row r="38" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="61"/>
       <c r="B38" s="15"/>
       <c r="C38" s="16" t="str">
@@ -3310,7 +3319,7 @@
       <c r="X38" s="14"/>
       <c r="Y38" s="14"/>
     </row>
-    <row r="39" spans="1:25" ht="16.5" thickTop="1">
+    <row r="39" spans="1:25" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A39" s="59"/>
       <c r="C39" s="5" t="str">
         <f>IFERROR(VLOOKUP(B39,#REF!,2,FALSE),"")</f>
@@ -3329,7 +3338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:25">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40" s="60"/>
       <c r="C40" s="5" t="str">
         <f>IFERROR(VLOOKUP(B40,#REF!,2,FALSE),"")</f>
@@ -3348,7 +3357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:25">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41" s="60"/>
       <c r="C41" s="5" t="str">
         <f>IFERROR(VLOOKUP(B41,#REF!,2,FALSE),"")</f>
@@ -3367,7 +3376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:25">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42" s="60"/>
       <c r="C42" s="5" t="str">
         <f>IFERROR(VLOOKUP(B42,#REF!,2,FALSE),"")</f>
@@ -3386,7 +3395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:25">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43" s="60"/>
       <c r="C43" s="5" t="str">
         <f>IFERROR(VLOOKUP(B43,#REF!,2,FALSE),"")</f>
@@ -3405,7 +3414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:25" ht="16.5" thickBot="1">
+    <row r="44" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="61"/>
       <c r="B44" s="15"/>
       <c r="C44" s="16" t="str">
@@ -3444,7 +3453,7 @@
       <c r="X44" s="14"/>
       <c r="Y44" s="14"/>
     </row>
-    <row r="45" spans="1:25" ht="16.5" thickTop="1">
+    <row r="45" spans="1:25" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A45" s="59"/>
       <c r="C45" s="5" t="str">
         <f>IFERROR(VLOOKUP(B45,#REF!,2,FALSE),"")</f>
@@ -3463,7 +3472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" s="60"/>
       <c r="C46" s="5" t="str">
         <f>IFERROR(VLOOKUP(B46,#REF!,2,FALSE),"")</f>
@@ -3482,7 +3491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47" s="60"/>
       <c r="C47" s="5" t="str">
         <f>IFERROR(VLOOKUP(B47,#REF!,2,FALSE),"")</f>
@@ -3501,7 +3510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:25">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A48" s="60"/>
       <c r="C48" s="5" t="str">
         <f>IFERROR(VLOOKUP(B48,#REF!,2,FALSE),"")</f>
@@ -3520,7 +3529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:25">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A49" s="60"/>
       <c r="C49" s="5" t="str">
         <f>IFERROR(VLOOKUP(B49,#REF!,2,FALSE),"")</f>
@@ -3539,7 +3548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:25" ht="16.5" thickBot="1">
+    <row r="50" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="61"/>
       <c r="B50" s="15"/>
       <c r="C50" s="16" t="str">
@@ -3578,7 +3587,7 @@
       <c r="X50" s="14"/>
       <c r="Y50" s="14"/>
     </row>
-    <row r="51" spans="1:25" ht="16.5" thickTop="1">
+    <row r="51" spans="1:25" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A51" s="59"/>
       <c r="C51" s="5" t="str">
         <f>IFERROR(VLOOKUP(B51,#REF!,2,FALSE),"")</f>
@@ -3597,7 +3606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:25">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A52" s="60"/>
       <c r="C52" s="5" t="str">
         <f>IFERROR(VLOOKUP(B52,#REF!,2,FALSE),"")</f>
@@ -3616,7 +3625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:25">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A53" s="60"/>
       <c r="C53" s="5" t="str">
         <f>IFERROR(VLOOKUP(B53,#REF!,2,FALSE),"")</f>
@@ -3635,7 +3644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:25">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A54" s="60"/>
       <c r="C54" s="5" t="str">
         <f>IFERROR(VLOOKUP(B54,#REF!,2,FALSE),"")</f>
@@ -3654,7 +3663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:25">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A55" s="60"/>
       <c r="C55" s="5" t="str">
         <f>IFERROR(VLOOKUP(B55,#REF!,2,FALSE),"")</f>
@@ -3673,7 +3682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:25" ht="16.5" thickBot="1">
+    <row r="56" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="61"/>
       <c r="B56" s="15"/>
       <c r="C56" s="16" t="str">
@@ -3712,7 +3721,7 @@
       <c r="X56" s="14"/>
       <c r="Y56" s="14"/>
     </row>
-    <row r="57" spans="1:25" ht="16.5" thickTop="1">
+    <row r="57" spans="1:25" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A57" s="59"/>
       <c r="C57" s="5" t="str">
         <f>IFERROR(VLOOKUP(B57,#REF!,2,FALSE),"")</f>
@@ -3731,7 +3740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:25">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A58" s="60"/>
       <c r="C58" s="5" t="str">
         <f>IFERROR(VLOOKUP(B58,#REF!,2,FALSE),"")</f>
@@ -3750,7 +3759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:25">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A59" s="60"/>
       <c r="C59" s="5" t="str">
         <f>IFERROR(VLOOKUP(B59,#REF!,2,FALSE),"")</f>
@@ -3769,7 +3778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:25">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A60" s="60"/>
       <c r="C60" s="5" t="str">
         <f>IFERROR(VLOOKUP(B60,#REF!,2,FALSE),"")</f>
@@ -3788,7 +3797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:25">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A61" s="60"/>
       <c r="C61" s="5" t="str">
         <f>IFERROR(VLOOKUP(B61,#REF!,2,FALSE),"")</f>
@@ -3807,7 +3816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:25" ht="16.5" thickBot="1">
+    <row r="62" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="61"/>
       <c r="B62" s="15"/>
       <c r="C62" s="16" t="str">
@@ -3846,7 +3855,7 @@
       <c r="X62" s="14"/>
       <c r="Y62" s="14"/>
     </row>
-    <row r="63" spans="1:25" ht="16.5" thickTop="1">
+    <row r="63" spans="1:25" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A63" s="59"/>
       <c r="C63" s="5" t="str">
         <f>IFERROR(VLOOKUP(B63,#REF!,2,FALSE),"")</f>
@@ -3865,7 +3874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:25">
+    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A64" s="60"/>
       <c r="C64" s="5" t="str">
         <f>IFERROR(VLOOKUP(B64,#REF!,2,FALSE),"")</f>
@@ -3884,7 +3893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:25">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A65" s="60"/>
       <c r="C65" s="5" t="str">
         <f>IFERROR(VLOOKUP(B65,#REF!,2,FALSE),"")</f>
@@ -3903,7 +3912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:25">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A66" s="60"/>
       <c r="C66" s="5" t="str">
         <f>IFERROR(VLOOKUP(B66,#REF!,2,FALSE),"")</f>
@@ -3922,7 +3931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:25">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A67" s="60"/>
       <c r="C67" s="5" t="str">
         <f>IFERROR(VLOOKUP(B67,#REF!,2,FALSE),"")</f>
@@ -3941,7 +3950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:25" ht="16.5" thickBot="1">
+    <row r="68" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="61"/>
       <c r="B68" s="15"/>
       <c r="C68" s="16" t="str">
@@ -3980,7 +3989,7 @@
       <c r="X68" s="14"/>
       <c r="Y68" s="14"/>
     </row>
-    <row r="69" spans="1:25" ht="16.5" thickTop="1">
+    <row r="69" spans="1:25" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A69" s="59"/>
       <c r="C69" s="5" t="str">
         <f>IFERROR(VLOOKUP(B69,#REF!,2,FALSE),"")</f>
@@ -3999,7 +4008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:25">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A70" s="60"/>
       <c r="C70" s="5" t="str">
         <f>IFERROR(VLOOKUP(B70,#REF!,2,FALSE),"")</f>
@@ -4018,7 +4027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:25">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A71" s="60"/>
       <c r="C71" s="5" t="str">
         <f>IFERROR(VLOOKUP(B71,#REF!,2,FALSE),"")</f>
@@ -4037,7 +4046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:25">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A72" s="60"/>
       <c r="C72" s="5" t="str">
         <f>IFERROR(VLOOKUP(B72,#REF!,2,FALSE),"")</f>
@@ -4056,7 +4065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:25">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A73" s="60"/>
       <c r="C73" s="5" t="str">
         <f>IFERROR(VLOOKUP(B73,#REF!,2,FALSE),"")</f>
@@ -4075,7 +4084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:25" ht="16.5" thickBot="1">
+    <row r="74" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="61"/>
       <c r="B74" s="15"/>
       <c r="C74" s="16" t="str">
@@ -4114,7 +4123,7 @@
       <c r="X74" s="14"/>
       <c r="Y74" s="14"/>
     </row>
-    <row r="75" spans="1:25" ht="16.5" thickTop="1">
+    <row r="75" spans="1:25" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A75" s="59"/>
       <c r="C75" s="5" t="str">
         <f>IFERROR(VLOOKUP(B75,#REF!,2,FALSE),"")</f>
@@ -4133,7 +4142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:25">
+    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A76" s="60"/>
       <c r="C76" s="5" t="str">
         <f>IFERROR(VLOOKUP(B76,#REF!,2,FALSE),"")</f>
@@ -4152,7 +4161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:25">
+    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A77" s="60"/>
       <c r="C77" s="5" t="str">
         <f>IFERROR(VLOOKUP(B77,#REF!,2,FALSE),"")</f>
@@ -4171,7 +4180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:25">
+    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A78" s="60"/>
       <c r="C78" s="5" t="str">
         <f>IFERROR(VLOOKUP(B78,#REF!,2,FALSE),"")</f>
@@ -4190,7 +4199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:25">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A79" s="60"/>
       <c r="C79" s="5" t="str">
         <f>IFERROR(VLOOKUP(B79,#REF!,2,FALSE),"")</f>
@@ -4209,7 +4218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:25" ht="16.5" thickBot="1">
+    <row r="80" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="61"/>
       <c r="B80" s="15"/>
       <c r="C80" s="16" t="str">
@@ -4248,7 +4257,7 @@
       <c r="X80" s="14"/>
       <c r="Y80" s="14"/>
     </row>
-    <row r="81" spans="1:25" ht="16.5" thickTop="1">
+    <row r="81" spans="1:25" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A81" s="59"/>
       <c r="C81" s="5" t="str">
         <f>IFERROR(VLOOKUP(B81,#REF!,2,FALSE),"")</f>
@@ -4267,7 +4276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:25">
+    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A82" s="60"/>
       <c r="C82" s="5" t="str">
         <f>IFERROR(VLOOKUP(B82,#REF!,2,FALSE),"")</f>
@@ -4286,7 +4295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:25">
+    <row r="83" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A83" s="60"/>
       <c r="C83" s="5" t="str">
         <f>IFERROR(VLOOKUP(B83,#REF!,2,FALSE),"")</f>
@@ -4305,7 +4314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:25">
+    <row r="84" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A84" s="60"/>
       <c r="C84" s="5" t="str">
         <f>IFERROR(VLOOKUP(B84,#REF!,2,FALSE),"")</f>
@@ -4324,7 +4333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:25">
+    <row r="85" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A85" s="60"/>
       <c r="C85" s="5" t="str">
         <f>IFERROR(VLOOKUP(B85,#REF!,2,FALSE),"")</f>
@@ -4343,7 +4352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:25" ht="16.5" thickBot="1">
+    <row r="86" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="61"/>
       <c r="B86" s="15"/>
       <c r="C86" s="16" t="str">
@@ -4382,7 +4391,7 @@
       <c r="X86" s="14"/>
       <c r="Y86" s="14"/>
     </row>
-    <row r="87" spans="1:25" ht="16.5" thickTop="1">
+    <row r="87" spans="1:25" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A87" s="59"/>
       <c r="C87" s="5" t="str">
         <f>IFERROR(VLOOKUP(B87,#REF!,2,FALSE),"")</f>
@@ -4401,7 +4410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:25">
+    <row r="88" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A88" s="60"/>
       <c r="C88" s="5" t="str">
         <f>IFERROR(VLOOKUP(B88,#REF!,2,FALSE),"")</f>
@@ -4420,7 +4429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:25">
+    <row r="89" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A89" s="60"/>
       <c r="C89" s="5" t="str">
         <f>IFERROR(VLOOKUP(B89,#REF!,2,FALSE),"")</f>
@@ -4439,7 +4448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:25">
+    <row r="90" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A90" s="60"/>
       <c r="C90" s="5" t="str">
         <f>IFERROR(VLOOKUP(B90,#REF!,2,FALSE),"")</f>
@@ -4458,7 +4467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:25">
+    <row r="91" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A91" s="60"/>
       <c r="C91" s="5" t="str">
         <f>IFERROR(VLOOKUP(B91,#REF!,2,FALSE),"")</f>
@@ -4477,7 +4486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:25" ht="16.5" thickBot="1">
+    <row r="92" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="61"/>
       <c r="B92" s="15"/>
       <c r="C92" s="16" t="str">
@@ -4516,7 +4525,7 @@
       <c r="X92" s="14"/>
       <c r="Y92" s="14"/>
     </row>
-    <row r="93" spans="1:25" ht="16.5" thickTop="1">
+    <row r="93" spans="1:25" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A93" s="59"/>
       <c r="C93" s="5" t="str">
         <f>IFERROR(VLOOKUP(B93,#REF!,2,FALSE),"")</f>
@@ -4535,7 +4544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:25">
+    <row r="94" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A94" s="60"/>
       <c r="C94" s="5" t="str">
         <f>IFERROR(VLOOKUP(B94,#REF!,2,FALSE),"")</f>
@@ -4554,7 +4563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:25">
+    <row r="95" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A95" s="60"/>
       <c r="C95" s="5" t="str">
         <f>IFERROR(VLOOKUP(B95,#REF!,2,FALSE),"")</f>
@@ -4573,7 +4582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:25">
+    <row r="96" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A96" s="60"/>
       <c r="C96" s="5" t="str">
         <f>IFERROR(VLOOKUP(B96,#REF!,2,FALSE),"")</f>
@@ -4592,7 +4601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:25">
+    <row r="97" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A97" s="60"/>
       <c r="C97" s="5" t="str">
         <f>IFERROR(VLOOKUP(B97,#REF!,2,FALSE),"")</f>
@@ -4611,7 +4620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:25" ht="16.5" thickBot="1">
+    <row r="98" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="61"/>
       <c r="B98" s="15"/>
       <c r="C98" s="16" t="str">
@@ -4650,7 +4659,7 @@
       <c r="X98" s="14"/>
       <c r="Y98" s="14"/>
     </row>
-    <row r="99" spans="1:25" ht="16.5" thickTop="1">
+    <row r="99" spans="1:25" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A99" s="59"/>
       <c r="C99" s="5" t="str">
         <f>IFERROR(VLOOKUP(B99,#REF!,2,FALSE),"")</f>
@@ -4669,7 +4678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:25">
+    <row r="100" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A100" s="60"/>
       <c r="C100" s="5" t="str">
         <f>IFERROR(VLOOKUP(B100,#REF!,2,FALSE),"")</f>
@@ -4688,7 +4697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:25">
+    <row r="101" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A101" s="60"/>
       <c r="C101" s="5" t="str">
         <f>IFERROR(VLOOKUP(B101,#REF!,2,FALSE),"")</f>
@@ -4707,7 +4716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:25">
+    <row r="102" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A102" s="60"/>
       <c r="C102" s="5" t="str">
         <f>IFERROR(VLOOKUP(B102,#REF!,2,FALSE),"")</f>
@@ -4726,7 +4735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:25">
+    <row r="103" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A103" s="60"/>
       <c r="C103" s="5" t="str">
         <f>IFERROR(VLOOKUP(B103,#REF!,2,FALSE),"")</f>
@@ -4745,7 +4754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:25" ht="16.5" thickBot="1">
+    <row r="104" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="61"/>
       <c r="B104" s="15"/>
       <c r="C104" s="16" t="str">
@@ -4784,7 +4793,7 @@
       <c r="X104" s="14"/>
       <c r="Y104" s="14"/>
     </row>
-    <row r="105" spans="1:25" ht="16.5" thickTop="1">
+    <row r="105" spans="1:25" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A105" s="59"/>
       <c r="C105" s="5" t="str">
         <f>IFERROR(VLOOKUP(B105,#REF!,2,FALSE),"")</f>
@@ -4803,7 +4812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:25">
+    <row r="106" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A106" s="60"/>
       <c r="C106" s="5" t="str">
         <f>IFERROR(VLOOKUP(B106,#REF!,2,FALSE),"")</f>
@@ -4822,7 +4831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:25">
+    <row r="107" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A107" s="60"/>
       <c r="C107" s="5" t="str">
         <f>IFERROR(VLOOKUP(B107,#REF!,2,FALSE),"")</f>
@@ -4841,7 +4850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:25">
+    <row r="108" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A108" s="60"/>
       <c r="C108" s="5" t="str">
         <f>IFERROR(VLOOKUP(B108,#REF!,2,FALSE),"")</f>
@@ -4860,7 +4869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:25">
+    <row r="109" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A109" s="60"/>
       <c r="C109" s="5" t="str">
         <f>IFERROR(VLOOKUP(B109,#REF!,2,FALSE),"")</f>
@@ -4879,7 +4888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:25" ht="16.5" thickBot="1">
+    <row r="110" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="61"/>
       <c r="B110" s="15"/>
       <c r="C110" s="16" t="str">
@@ -4918,7 +4927,7 @@
       <c r="X110" s="14"/>
       <c r="Y110" s="14"/>
     </row>
-    <row r="111" spans="1:25" ht="16.5" thickTop="1">
+    <row r="111" spans="1:25" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A111" s="59"/>
       <c r="C111" s="5" t="str">
         <f>IFERROR(VLOOKUP(B111,#REF!,2,FALSE),"")</f>
@@ -4937,7 +4946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:25">
+    <row r="112" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A112" s="60"/>
       <c r="C112" s="5" t="str">
         <f>IFERROR(VLOOKUP(B112,#REF!,2,FALSE),"")</f>
@@ -4956,7 +4965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:25">
+    <row r="113" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A113" s="60"/>
       <c r="C113" s="5" t="str">
         <f>IFERROR(VLOOKUP(B113,#REF!,2,FALSE),"")</f>
@@ -4975,7 +4984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:25">
+    <row r="114" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A114" s="60"/>
       <c r="C114" s="5" t="str">
         <f>IFERROR(VLOOKUP(B114,#REF!,2,FALSE),"")</f>
@@ -4994,7 +5003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:25">
+    <row r="115" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A115" s="60"/>
       <c r="C115" s="5" t="str">
         <f>IFERROR(VLOOKUP(B115,#REF!,2,FALSE),"")</f>
@@ -5013,7 +5022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:25" ht="16.5" thickBot="1">
+    <row r="116" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="61"/>
       <c r="B116" s="15"/>
       <c r="C116" s="16" t="str">
@@ -5052,7 +5061,7 @@
       <c r="X116" s="14"/>
       <c r="Y116" s="14"/>
     </row>
-    <row r="117" spans="1:25" ht="16.5" thickTop="1">
+    <row r="117" spans="1:25" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A117" s="59"/>
       <c r="C117" s="5" t="str">
         <f>IFERROR(VLOOKUP(B117,#REF!,2,FALSE),"")</f>
@@ -5071,7 +5080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:25">
+    <row r="118" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A118" s="60"/>
       <c r="C118" s="5" t="str">
         <f>IFERROR(VLOOKUP(B118,#REF!,2,FALSE),"")</f>
@@ -5090,7 +5099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:25">
+    <row r="119" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A119" s="60"/>
       <c r="C119" s="5" t="str">
         <f>IFERROR(VLOOKUP(B119,#REF!,2,FALSE),"")</f>
@@ -5109,7 +5118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:25">
+    <row r="120" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A120" s="60"/>
       <c r="C120" s="5" t="str">
         <f>IFERROR(VLOOKUP(B120,#REF!,2,FALSE),"")</f>
@@ -5128,7 +5137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:25">
+    <row r="121" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A121" s="60"/>
       <c r="C121" s="5" t="str">
         <f>IFERROR(VLOOKUP(B121,#REF!,2,FALSE),"")</f>
@@ -5147,7 +5156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:25" ht="16.5" thickBot="1">
+    <row r="122" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="61"/>
       <c r="B122" s="15"/>
       <c r="C122" s="16" t="str">
@@ -5186,17 +5195,9 @@
       <c r="X122" s="14"/>
       <c r="Y122" s="14"/>
     </row>
-    <row r="123" spans="1:25" ht="16.5" thickTop="1"/>
+    <row r="123" spans="1:25" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A111:A116"/>
-    <mergeCell ref="A117:A122"/>
-    <mergeCell ref="A75:A80"/>
-    <mergeCell ref="A81:A86"/>
-    <mergeCell ref="A87:A92"/>
-    <mergeCell ref="A93:A98"/>
-    <mergeCell ref="A99:A104"/>
-    <mergeCell ref="A105:A110"/>
     <mergeCell ref="A69:A74"/>
     <mergeCell ref="A3:A8"/>
     <mergeCell ref="A9:A14"/>
@@ -5209,6 +5210,14 @@
     <mergeCell ref="A51:A56"/>
     <mergeCell ref="A57:A62"/>
     <mergeCell ref="A63:A68"/>
+    <mergeCell ref="A111:A116"/>
+    <mergeCell ref="A117:A122"/>
+    <mergeCell ref="A75:A80"/>
+    <mergeCell ref="A81:A86"/>
+    <mergeCell ref="A87:A92"/>
+    <mergeCell ref="A93:A98"/>
+    <mergeCell ref="A99:A104"/>
+    <mergeCell ref="A105:A110"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="Erro de Avaliação" error="A avaliação deve ser realizada na escala de 0 (zero) a 5 (cinco). _x000a_Pode usar valores com casas decimais (e.g. &quot;3.5&quot;)." sqref="E3:T1218" xr:uid="{FCA5644E-B2E5-F346-99E2-8E50061E9E9E}">
@@ -5217,34 +5226,11 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="79ce0200-2809-4097-82e4-fb85aa45ded7">
-      <UserInfo>
-        <DisplayName>ESOFT 2021-2022 Docentes-ISEP365Group Members</DisplayName>
-        <AccountId>8</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008745C7147682F4439D59E4AED2659347" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3a274f58fe90dd6afd9684e487978f4f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e879a7a9-e2e4-465e-90fc-6738fa56acd3" xmlns:ns3="79ce0200-2809-4097-82e4-fb85aa45ded7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3599ba8e0dd80460426f652f1588fe87" ns2:_="" ns3:_="">
     <xsd:import namespace="e879a7a9-e2e4-465e-90fc-6738fa56acd3"/>
@@ -5435,14 +5421,62 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="79ce0200-2809-4097-82e4-fb85aa45ded7">
+      <UserInfo>
+        <DisplayName>ESOFT 2021-2022 Docentes-ISEP365Group Members</DisplayName>
+        <AccountId>8</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{565285F7-F5B7-459C-A043-A383F1753FE1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{861BA5EF-48E9-4E0A-AA41-B56B83E3E13A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e879a7a9-e2e4-465e-90fc-6738fa56acd3"/>
+    <ds:schemaRef ds:uri="79ce0200-2809-4097-82e4-fb85aa45ded7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{593F2428-6100-4200-B62E-EA3F22E68287}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{593F2428-6100-4200-B62E-EA3F22E68287}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{861BA5EF-48E9-4E0A-AA41-B56B83E3E13A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{565285F7-F5B7-459C-A043-A383F1753FE1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="79ce0200-2809-4097-82e4-fb85aa45ded7"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>